<commit_message>
Add 'red cross' 'red crescent' org in other lang
</commit_message>
<xml_diff>
--- a/RCRC GitHub Organizations.xlsx
+++ b/RCRC GitHub Organizations.xlsx
@@ -8,13 +8,13 @@
     <sheet state="visible" name="all_org" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="1" name="Z_C6C9B2FC_A6FC_407B_AB15_3DD46B6BC3E2_.wvu.FilterData">ns_org!$E$1:$E$1002</definedName>
-    <definedName hidden="1" localSheetId="1" name="Z_B1F8ED39_6270_438E_BF9E_7109FC9791AA_.wvu.FilterData">ns_org!$F$1:$F$1002</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_F74AAE41_3595_4B2B_B07C_FDF6C1A59922_.wvu.FilterData">ns_org!$F$1:$F$1002</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_40F0C144_3C06_44C6_A638_8E0BA60BB579_.wvu.FilterData">ns_org!$E$1:$E$1002</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{B1F8ED39-6270-438E-BF9E-7109FC9791AA}" name="Filter 2"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{C6C9B2FC-A6FC-407B-AB15-3DD46B6BC3E2}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{F74AAE41-3595-4B2B-B07C-FDF6C1A59922}" name="Filter 2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{40F0C144-3C06-44C6-A638-8E0BA60BB579}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -63,12 +63,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="524">
   <si>
     <r>
       <rPr/>
       <t xml:space="preserve">Hi there!
-After a loose search of GitHub Organizations with the 'red cross' and 'red crescent' terms in their names on October 27th of 2022, we have created a list of organizations that we think might contain repositories of our collective interest. 
+After a loose search of GitHub Organizations with the red cross and red crescent terms in their names from October 27th of 2022 to January 20th of 2023, we have created a list of organizations that we think might contain repositories of our collective interest. 
 We haven't been able to verify those organizations/accounts. But we are in the process of doing that, starting by asking the </t>
     </r>
     <r>
@@ -80,7 +80,7 @@
     </r>
     <r>
       <rPr/>
-      <t xml:space="preserve">. We also know that we need to widen our search, as there are some RCRC organizations with their names in their local language. The inclusion of those organizations is also envisioned as a next step.
+      <t xml:space="preserve">. 
 Please </t>
     </r>
     <r>
@@ -219,7 +219,7 @@
     <t>Ethiopia</t>
   </si>
   <si>
-    <t>Ethopia Red Cross</t>
+    <t>Ethiopia Red Cross</t>
   </si>
   <si>
     <t>Gabon</t>
@@ -612,7 +612,7 @@
     <t xml:space="preserve">Uruguay </t>
   </si>
   <si>
-    <t xml:space="preserve">Uruguyan Red Cross </t>
+    <t xml:space="preserve">Uruguayan Red Cross </t>
   </si>
   <si>
     <t xml:space="preserve">Venezuela </t>
@@ -1300,9 +1300,6 @@
   </si>
   <si>
     <t>Top Languages</t>
-  </si>
-  <si>
-    <t>Authentic</t>
   </si>
   <si>
     <t>Netherlands Red Cross</t>
@@ -1681,6 +1678,12 @@
     <t>Croce Rossa Italiana - Catania</t>
   </si>
   <si>
+    <t>Croce Rossa Molfetta</t>
+  </si>
+  <si>
+    <t>Croce Rossa Italiana - Gruppo di Lavis</t>
+  </si>
+  <si>
     <t>Canadian Red Cross</t>
   </si>
   <si>
@@ -1823,6 +1826,90 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>Cruz Roja Española</t>
+  </si>
+  <si>
+    <t>Web App, Resources</t>
+  </si>
+  <si>
+    <t>Cruz Roja Uruguaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uruguyan Red Cross </t>
+  </si>
+  <si>
+    <t>Cruz Roja en La Rioja</t>
+  </si>
+  <si>
+    <t>Cruz Roja Holandesa en Guatemala</t>
+  </si>
+  <si>
+    <t>Web App</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>Cruz Roja Ecuatoriana - Tecnologías de la Información</t>
+  </si>
+  <si>
+    <t>Croix-Rouge française 95</t>
+  </si>
+  <si>
+    <t>Croix Rouge Jeunesse</t>
+  </si>
+  <si>
+    <t>Croix-Rouge française de Paris</t>
+  </si>
+  <si>
+    <t>Croix Rouge Française - Minutis/Redcall</t>
+  </si>
+  <si>
+    <t>Web App, Data Analysis, Data Acquisition</t>
+  </si>
+  <si>
+    <t>PHP, jQuery, Bootstrap</t>
+  </si>
+  <si>
+    <t>Croix-Rouge Française - Délégation locale de Paris III et X</t>
+  </si>
+  <si>
+    <t>Cruz Vermelha - Coordenação Nacional de Emergência</t>
+  </si>
+  <si>
+    <t>Web app, Data Analysis, Data Acquisition</t>
+  </si>
+  <si>
+    <t>Cruz Vermelha Portuguesa - Delegação Faro-Loulé</t>
+  </si>
+  <si>
+    <t>Youth Red Cross, SJCE</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>Österreichisches Rotes Kreuz</t>
+  </si>
+  <si>
+    <t>Mobile app, Web app, Resources</t>
+  </si>
+  <si>
+    <t>Java, Kotlin, Swift</t>
+  </si>
+  <si>
+    <t>Deutsches Rotes Kreuz Kreis Euskirchen</t>
+  </si>
+  <si>
+    <t>Deutsches Rotes Kreuz Kreisverband Groß-Gerau e.V.</t>
+  </si>
+  <si>
+    <t>Rotes Kreuz</t>
+  </si>
+  <si>
+    <t>Rode Kruis Vlaams-Brabant</t>
   </si>
 </sst>
 </file>
@@ -1946,7 +2033,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1976,6 +2063,9 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -2607,7 +2697,7 @@
       <c r="B18" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="6"/>
@@ -3316,10 +3406,18 @@
       <c r="C64" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D64" s="6"/>
-      <c r="E64" s="6"/>
-      <c r="F64" s="6"/>
-      <c r="G64" s="6"/>
+      <c r="D64" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="E64" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="F64" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="G64" s="9">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
@@ -3606,13 +3704,21 @@
       <c r="B83" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C83" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="D83" s="6"/>
-      <c r="E83" s="6"/>
-      <c r="F83" s="6"/>
-      <c r="G83" s="6"/>
+      <c r="D83" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="E83" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="F83" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="G83" s="9">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="5" t="s">
@@ -3812,10 +3918,18 @@
       <c r="C96" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D96" s="6"/>
-      <c r="E96" s="6"/>
-      <c r="F96" s="6"/>
-      <c r="G96" s="6"/>
+      <c r="D96" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E96" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F96" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="G96" s="9">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="5" t="s">
@@ -3970,10 +4084,18 @@
       <c r="C106" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="D106" s="6"/>
-      <c r="E106" s="6"/>
-      <c r="F106" s="6"/>
-      <c r="G106" s="6"/>
+      <c r="D106" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E106" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="F106" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="G106" s="9">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="5" t="s">
@@ -4286,10 +4408,18 @@
       <c r="C126" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="D126" s="6"/>
-      <c r="E126" s="6"/>
-      <c r="F126" s="6"/>
-      <c r="G126" s="6"/>
+      <c r="D126" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E126" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="F126" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="G126" s="9">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="5" t="s">
@@ -4490,10 +4620,18 @@
       <c r="C138" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="D138" s="6"/>
-      <c r="E138" s="6"/>
-      <c r="F138" s="6"/>
-      <c r="G138" s="6"/>
+      <c r="D138" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E138" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F138" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="G138" s="9">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="5" t="s">
@@ -4520,10 +4658,18 @@
       <c r="C140" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="D140" s="6"/>
-      <c r="E140" s="6"/>
-      <c r="F140" s="6"/>
-      <c r="G140" s="6"/>
+      <c r="D140" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="E140" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F140" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="G140" s="9">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="5" t="s">
@@ -4772,7 +4918,7 @@
         <v>1.0</v>
       </c>
       <c r="E156" s="9">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F156" s="9">
         <v>1.0</v>
@@ -4788,7 +4934,7 @@
       <c r="B157" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="C157" s="5" t="s">
+      <c r="C157" s="10" t="s">
         <v>323</v>
       </c>
       <c r="D157" s="9">
@@ -4829,10 +4975,18 @@
       <c r="C159" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="D159" s="6"/>
-      <c r="E159" s="6"/>
-      <c r="F159" s="6"/>
-      <c r="G159" s="6"/>
+      <c r="D159" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E159" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F159" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="G159" s="9">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="5" t="s">
@@ -4964,10 +5118,18 @@
       <c r="C168" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="D168" s="6"/>
-      <c r="E168" s="6"/>
-      <c r="F168" s="6"/>
-      <c r="G168" s="6"/>
+      <c r="D168" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E168" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F168" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="G168" s="9">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="5" t="s">
@@ -5394,7 +5556,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B1F8ED39-6270-438E-BF9E-7109FC9791AA}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{F74AAE41-3595-4B2B-B07C-FDF6C1A59922}" filter="1" showAutoFilter="1">
       <autoFilter ref="$F$1:$F$1002">
         <filterColumn colId="0">
           <filters>
@@ -5403,7 +5565,7 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{C6C9B2FC-A6FC-407B-AB15-3DD46B6BC3E2}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{40F0C144-3C06-44C6-A638-8E0BA60BB579}" filter="1" showAutoFilter="1">
       <autoFilter ref="$E$1:$E$1002"/>
     </customSheetView>
   </customSheetViews>
@@ -5421,11 +5583,14 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="38.75"/>
+    <col customWidth="1" min="1" max="1" width="45.13"/>
     <col customWidth="1" min="2" max="3" width="29.0"/>
     <col customWidth="1" min="4" max="4" width="15.75"/>
     <col customWidth="1" min="5" max="5" width="19.75"/>
@@ -5454,13 +5619,10 @@
       <c r="G1" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="H1" s="4" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="11" t="s">
         <v>403</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="10" t="s">
-        <v>404</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>321</v>
@@ -5474,16 +5636,16 @@
       <c r="E2" s="2">
         <v>114.0</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="12" t="s">
+        <v>404</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="G2" s="2" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="13" t="s">
         <v>406</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="12" t="s">
-        <v>407</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>359</v>
@@ -5497,16 +5659,16 @@
       <c r="E3" s="2">
         <v>26.0</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="12" t="s">
+        <v>407</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>408</v>
       </c>
-      <c r="G3" s="13" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="15" t="s">
         <v>409</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="14" t="s">
-        <v>410</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>359</v>
@@ -5522,11 +5684,11 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>411</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>412</v>
       </c>
       <c r="D5" s="2">
         <v>0.0</v>
@@ -5535,29 +5697,29 @@
         <v>8.0</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="G5" s="13" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="16" t="s">
         <v>414</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="15" t="s">
-        <v>411</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="15" t="s">
-        <v>415</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>171</v>
@@ -5571,16 +5733,16 @@
       <c r="E7" s="2">
         <v>150.0</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="12" t="s">
+        <v>415</v>
+      </c>
+      <c r="G7" s="17" t="s">
         <v>416</v>
       </c>
-      <c r="G7" s="16" t="s">
+    </row>
+    <row r="8">
+      <c r="A8" s="16" t="s">
         <v>417</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="15" t="s">
-        <v>418</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>171</v>
@@ -5593,15 +5755,15 @@
         <v>11.0</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="G8" s="14" t="s">
         <v>419</v>
       </c>
-      <c r="G8" s="13" t="s">
+    </row>
+    <row r="9">
+      <c r="A9" s="16" t="s">
         <v>420</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="15" t="s">
-        <v>421</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>171</v>
@@ -5614,15 +5776,15 @@
         <v>1.0</v>
       </c>
       <c r="F9" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="G9" s="2" t="s">
+    </row>
+    <row r="10">
+      <c r="A10" s="16" t="s">
         <v>423</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="15" t="s">
-        <v>424</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>171</v>
@@ -5635,15 +5797,15 @@
         <v>1.0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="16" t="s">
         <v>425</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="15" t="s">
-        <v>426</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>171</v>
@@ -5656,15 +5818,15 @@
         <v>1.0</v>
       </c>
       <c r="F11" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="G11" s="2" t="s">
+    </row>
+    <row r="12">
+      <c r="A12" s="16" t="s">
         <v>428</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="15" t="s">
-        <v>429</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>171</v>
@@ -5678,8 +5840,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="15" t="s">
-        <v>430</v>
+      <c r="A13" s="16" t="s">
+        <v>429</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>228</v>
@@ -5693,7 +5855,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="15" t="s">
         <v>228</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -5707,15 +5869,15 @@
         <v>48.0</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="G14" s="14" t="s">
         <v>431</v>
       </c>
-      <c r="G14" s="13" t="s">
+    </row>
+    <row r="15">
+      <c r="A15" s="16" t="s">
         <v>432</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="15" t="s">
-        <v>433</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>228</v>
@@ -5728,15 +5890,15 @@
         <v>1.0</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G15" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="16" t="s">
         <v>434</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="15" t="s">
-        <v>435</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>355</v>
@@ -5749,15 +5911,15 @@
         <v>1.0</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="G16" s="2" t="s">
+    </row>
+    <row r="17">
+      <c r="A17" s="16" t="s">
         <v>437</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="15" t="s">
-        <v>438</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>202</v>
@@ -5770,12 +5932,12 @@
         <v>12.0</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="16" t="s">
         <v>439</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="15" t="s">
-        <v>440</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>283</v>
@@ -5788,14 +5950,14 @@
         <v>22.0</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>441</v>
+        <v>426</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="16" t="s">
         <v>349</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -5809,15 +5971,15 @@
         <v>8.0</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="G19" s="13" t="s">
+        <v>438</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="16" t="s">
         <v>442</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="15" t="s">
-        <v>443</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>301</v>
@@ -5830,15 +5992,15 @@
         <v>9.0</v>
       </c>
       <c r="F20" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="G20" s="17" t="s">
         <v>444</v>
       </c>
-      <c r="G20" s="16" t="s">
+    </row>
+    <row r="21">
+      <c r="A21" s="16" t="s">
         <v>445</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="15" t="s">
-        <v>446</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>301</v>
@@ -5851,72 +6013,70 @@
         <v>2.0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
-        <v>447</v>
+      <c r="A22" s="11" t="s">
+        <v>446</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>121</v>
+        <v>301</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="2">
         <v>1.0</v>
       </c>
       <c r="E22" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>449</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
     </row>
     <row r="23">
-      <c r="A23" s="10" t="s">
-        <v>450</v>
+      <c r="A23" s="11" t="s">
+        <v>447</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>121</v>
+        <v>301</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="2">
         <v>0.0</v>
       </c>
       <c r="E23" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>452</v>
-      </c>
+        <v>2.0</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
     </row>
     <row r="24">
-      <c r="A24" s="15" t="s">
-        <v>453</v>
+      <c r="A24" s="16" t="s">
+        <v>448</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>121</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E24" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="10" t="s">
-        <v>454</v>
+      <c r="A25" s="11" t="s">
+        <v>451</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>121</v>
@@ -5926,12 +6086,18 @@
         <v>0.0</v>
       </c>
       <c r="E25" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="15" t="s">
-        <v>455</v>
+      <c r="A26" s="16" t="s">
+        <v>454</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>121</v>
@@ -5945,122 +6111,119 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="15" t="s">
-        <v>456</v>
+      <c r="A27" s="11" t="s">
+        <v>455</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>121</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E27" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="15" t="s">
-        <v>457</v>
+      <c r="A28" s="16" t="s">
+        <v>456</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>54</v>
+        <v>121</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="2">
         <v>0.0</v>
       </c>
       <c r="E28" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>458</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>449</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="10" t="s">
-        <v>459</v>
+      <c r="A29" s="16" t="s">
+        <v>457</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>224</v>
+        <v>121</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E29" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>461</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="15" t="s">
-        <v>462</v>
+      <c r="A30" s="16" t="s">
+        <v>458</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>390</v>
+        <v>54</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E30" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>463</v>
+        <v>1.0</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>459</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>464</v>
+        <v>450</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="12" t="s">
-        <v>279</v>
+      <c r="A31" s="11" t="s">
+        <v>460</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>279</v>
+        <v>224</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="2">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="E31" s="2">
-        <v>0.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="15" t="s">
-        <v>465</v>
+      <c r="A32" s="16" t="s">
+        <v>463</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>279</v>
+        <v>390</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E32" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>436</v>
+        <v>4.0</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="15" t="s">
-        <v>466</v>
+      <c r="A33" s="13" t="s">
+        <v>279</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="2">
@@ -6071,99 +6234,94 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="15" t="s">
-        <v>467</v>
+      <c r="A34" s="16" t="s">
+        <v>466</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>378</v>
+        <v>279</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="2">
         <v>0.0</v>
       </c>
       <c r="E34" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>468</v>
+        <v>2.0</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="15" t="s">
-        <v>469</v>
+      <c r="A35" s="16" t="s">
+        <v>467</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>180</v>
+        <v>269</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="2">
         <v>0.0</v>
       </c>
       <c r="E35" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="15" t="s">
-        <v>470</v>
+      <c r="A36" s="16" t="s">
+        <v>468</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>323</v>
+        <v>378</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="2">
         <v>0.0</v>
       </c>
       <c r="E36" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="15" t="s">
-        <v>471</v>
+      <c r="A37" s="16" t="s">
+        <v>470</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>357</v>
+        <v>180</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="2">
         <v>0.0</v>
       </c>
       <c r="E37" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="16" t="s">
         <v>472</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="C38" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D38" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E38" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>474</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="18" t="s">
-        <v>475</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="C39" s="2"/>
+      <c r="B39" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="C39" s="5"/>
       <c r="D39" s="2">
         <v>0.0</v>
       </c>
@@ -6173,205 +6331,565 @@
     </row>
     <row r="40">
       <c r="A40" s="18" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="C40" s="2"/>
+        <v>474</v>
+      </c>
+      <c r="C40" s="2">
+        <v>1.0</v>
+      </c>
       <c r="D40" s="2">
         <v>0.0</v>
       </c>
       <c r="E40" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="19" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2">
         <v>0.0</v>
       </c>
       <c r="E41" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>423</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="18" t="s">
-        <v>479</v>
+      <c r="A42" s="19" t="s">
+        <v>477</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2">
         <v>0.0</v>
       </c>
       <c r="E42" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="F42" s="2" t="s">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="20" t="s">
         <v>478</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="18" t="s">
-        <v>480</v>
-      </c>
       <c r="B43" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2">
         <v>0.0</v>
       </c>
       <c r="E43" s="2">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>458</v>
+        <v>479</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>481</v>
+        <v>422</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="18" t="s">
-        <v>482</v>
+      <c r="A44" s="19" t="s">
+        <v>480</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2">
         <v>0.0</v>
       </c>
       <c r="E44" s="2">
-        <v>11.0</v>
+        <v>4.0</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>484</v>
+        <v>422</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="19" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="C45" s="2">
-        <v>1.0</v>
-      </c>
+        <v>474</v>
+      </c>
+      <c r="C45" s="2"/>
       <c r="D45" s="2">
         <v>0.0</v>
       </c>
       <c r="E45" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="F45" s="11" t="s">
-        <v>436</v>
+        <v>7.0</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="19" t="s">
+        <v>483</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E46" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="20" t="s">
         <v>486</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="C46" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D46" s="2">
+      <c r="B47" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C47" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E47" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="20" t="s">
+        <v>487</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C48" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D48" s="2">
         <v>6.0</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E48" s="2">
         <v>65.0</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="G46" s="16" t="s">
+      <c r="F48" s="2" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="10" t="s">
-        <v>473</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E47" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="18" t="s">
+      <c r="G48" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="C48" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D48" s="2">
+    </row>
+    <row r="49">
+      <c r="A49" s="11" t="s">
+        <v>474</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E49" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="19" t="s">
+        <v>490</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C50" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D50" s="2">
         <v>2.0</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E50" s="2">
         <v>2.0</v>
       </c>
-      <c r="F48" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="G48" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="20" t="s">
+      <c r="G50" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="B49" s="5" t="s">
+    </row>
+    <row r="51">
+      <c r="A51" s="21" t="s">
+        <v>493</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="C49" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D49" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E49" s="2">
+      <c r="C51" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E51" s="2">
         <v>5.0</v>
       </c>
-      <c r="F49" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="G49" s="2" t="s">
+      <c r="F51" s="2" t="s">
         <v>494</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="11" t="s">
+        <v>496</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="D52" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="E52" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="11" t="s">
+        <v>498</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E53" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="11" t="s">
+        <v>500</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="D54" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E54" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="11" t="s">
+        <v>501</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E55" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E56" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="11" t="s">
+        <v>505</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E57" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="11" t="s">
+        <v>506</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E58" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="11" t="s">
+        <v>507</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E59" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="11" t="s">
+        <v>508</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D60" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E60" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="11" t="s">
+        <v>511</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D61" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E61" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="11" t="s">
+        <v>512</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E62" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>513</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="11" t="s">
+        <v>514</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="D63" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E63" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="11" t="s">
+        <v>515</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E64" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D65" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E65" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="11" t="s">
+        <v>517</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D66" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="E66" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="D67" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E67" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="11" t="s">
+        <v>521</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="D68" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E68" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="D69" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E69" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="D70" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E70" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D71" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E71" s="2">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -6412,9 +6930,9 @@
     <hyperlink r:id="rId35" ref="A27"/>
     <hyperlink r:id="rId36" ref="A28"/>
     <hyperlink r:id="rId37" ref="A29"/>
-    <hyperlink r:id="rId38" ref="G29"/>
-    <hyperlink r:id="rId39" ref="A30"/>
-    <hyperlink r:id="rId40" ref="A31"/>
+    <hyperlink r:id="rId38" ref="A30"/>
+    <hyperlink r:id="rId39" ref="A31"/>
+    <hyperlink r:id="rId40" ref="G31"/>
     <hyperlink r:id="rId41" ref="A32"/>
     <hyperlink r:id="rId42" ref="A33"/>
     <hyperlink r:id="rId43" ref="A34"/>
@@ -6430,12 +6948,34 @@
     <hyperlink r:id="rId53" ref="A44"/>
     <hyperlink r:id="rId54" ref="A45"/>
     <hyperlink r:id="rId55" ref="A46"/>
-    <hyperlink r:id="rId56" ref="G46"/>
-    <hyperlink r:id="rId57" ref="A47"/>
-    <hyperlink r:id="rId58" ref="A48"/>
+    <hyperlink r:id="rId56" ref="A47"/>
+    <hyperlink r:id="rId57" ref="A48"/>
+    <hyperlink r:id="rId58" ref="G48"/>
     <hyperlink r:id="rId59" ref="A49"/>
+    <hyperlink r:id="rId60" ref="A50"/>
+    <hyperlink r:id="rId61" ref="A51"/>
+    <hyperlink r:id="rId62" ref="A52"/>
+    <hyperlink r:id="rId63" ref="A53"/>
+    <hyperlink r:id="rId64" ref="A54"/>
+    <hyperlink r:id="rId65" ref="A55"/>
+    <hyperlink r:id="rId66" ref="A56"/>
+    <hyperlink r:id="rId67" ref="A57"/>
+    <hyperlink r:id="rId68" ref="A58"/>
+    <hyperlink r:id="rId69" ref="A59"/>
+    <hyperlink r:id="rId70" ref="A60"/>
+    <hyperlink r:id="rId71" ref="A61"/>
+    <hyperlink r:id="rId72" ref="A62"/>
+    <hyperlink r:id="rId73" ref="A63"/>
+    <hyperlink r:id="rId74" ref="A64"/>
+    <hyperlink r:id="rId75" ref="A65"/>
+    <hyperlink r:id="rId76" ref="A66"/>
+    <hyperlink r:id="rId77" ref="A67"/>
+    <hyperlink r:id="rId78" ref="A68"/>
+    <hyperlink r:id="rId79" ref="A69"/>
+    <hyperlink r:id="rId80" ref="A70"/>
+    <hyperlink r:id="rId81" ref="A71"/>
   </hyperlinks>
-  <drawing r:id="rId60"/>
-  <legacyDrawing r:id="rId61"/>
+  <drawing r:id="rId82"/>
+  <legacyDrawing r:id="rId83"/>
 </worksheet>
 </file>
</xml_diff>